<commit_message>
last runs with llama 3b and 1b
</commit_message>
<xml_diff>
--- a/model/src/rag_zero_shot_prompting_easy_Llama3B_results.xlsx
+++ b/model/src/rag_zero_shot_prompting_easy_Llama3B_results.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1176153\Downloads\github\Thesis\model\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3175109D-798D-4DD0-847F-1ED68C1B49BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB95B52-3272-4F04-9741-DEE5F8D51B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="157">
   <si>
     <t>question</t>
   </si>
@@ -293,42 +306,6 @@
   </si>
   <si>
     <t>What are the course units of the Spring semesters for the postgraduate program in risk analysis and management?</t>
-  </si>
-  <si>
-    <t>The course units for the Spring semester of the postgraduate program in Risk Analysis and Management are:
-* Banking and Insurance Regulation and Supervision (Mandatory, 7.5 ECTS)
-* Risk Management (Mandatory, 3.5 ECTS)
-* Financial Derivatives and Risk Management (Mandatory, 7.5 ECTS)
-* Market and Liquidity Risk Management (Mandatory, 4 ECTS)
-* Analysis of Discrete Data (Elective, 4 ECTS)
-* Analysis of Variance (Elective, 4 ECTS)
-* Architectures for Information Systems (Elective, 3.5 ECTS)
-* Big Data Analytics (Elective, 7.5 ECTS)
-* Blockchain (Elective, 4 ECTS)
-* Blockchain &amp; CryptoAssets (Elective, 4 ECTS)
-* Business Impact of Digital Projects (Elective, 3.5 ECTS)
-* Business Intelligence II (Elective, 7.5 ECTS)
-* Computational Statistics II (Elective, 6 ECTS)
-* Customer Relationship Management Systems (Elective, 7.5 ECTS)
-* Cybersecurity (Elective, 7.5 ECTS)
-* Data Mining II (Elective, 7.5 ECTS)
-* Data Visualization (Elective, 7.5 ECTS)
-* Data-driven decision making (Elective, 4 ECTS)
-* E-Business (Elective, 4 ECTS)
-* Econometrics Methods (Elective, 7.5 ECTS)
-* Emerging Technologies for Innovation (Elective, 3.5 ECTS)
-* Enterprise Cloud Mobility (Elective, 7.5 ECTS)
-* Financial Reporting (Elective, 6 ECTS)
-* Gestão do Conhecimento (Elective, 3.5 ECTS)
-* Industry 4.0 (Elective, 4 ECTS)
-* Information Project Management (Elective, 4 ECTS)
-* Innovation Management and Design Thinking (Elective, 7.5 ECTS)
-* Knowledge Management (Elective, 7.5 ECTS)
-* Leadership and People Management (Elective, 7.5 ECTS)
-* Process Mining Powered By Nokia (Elective, 7.5 ECTS)
-* Sampling Theory and Methods (Elective, 7.5 ECTS)
-* Smart and Sustainable Cities (Elective, 7.5 ECTS)
-Please note that this list only includes the course units for the Spring semester and does not include the course units for the other semesters. For a complete overview of the program, I recommend visiting the official course page.</t>
   </si>
   <si>
     <t>Document 1:
@@ -1113,21 +1090,6 @@
 Metadata: {'course_name': 'Postgraduate Program In Business Intelligence', 'degree': 'postgraduate', 'doc_type': 'study_plan', 'id': '8e619601-aa42-4c72-9c50-c2b40178f697', 'source': 'postgraduate-program-in-business-intelligence_Study plan.txt'}</t>
   </si>
   <si>
-    <t>What programming languages are taught in the Bachelor's in Data Science?</t>
-  </si>
-  <si>
-    <t>The programming languages taught in the Bachelor's in Data Science are Python and R. These languages are fundamental in the field of data science and are used extensively in data preprocessing, visualization, machine learning, and statistical inference. For more information, please visit the official course page for the Bachelor's in Data Science.</t>
-  </si>
-  <si>
-    <t>Document 1:
-Data Science bachelor What is the language of instruction of the course?
-The course is taught in English. Nowadays, being comfortable with the English language is a competitive advantage, which makes a difference in the global job market. NOVA IMS students have all the support to quickly adapt to the language and can always speak in Portuguese when they are unable to express themselves.
-Metadata: {'degree': 'bachelor', 'doc_type': 'main_info', 'course_name': 'Data Science', 'section': 'What is the language of instruction of the course?', 'id': 'fceef734-ee09-4571-b984-15a1216d9bc7'}
-Document 2:
-Data Science bachelor First Semester 2 nd year - Fall Semester Course Units Duration Type Contact Hours Total Workload ECTS Data preprocessing and visualization Semester Mandatory TP - 67,5 | OT - 7,5 168 6 Databases Semester Mandatory TP - 64,5 | S - 3 | OT - 7,5 168 6 Machine Learning I Semester Mandatory TP - 67,5 | OT - 7,5 168 6 Programming for Data Science Semester Mandatory TP - 67,5 | OT - 7,5 168 6 Statistical Inference Semester Mandatory TP - 67,5 | OT - 7,5 168 6 Show subtitles T – Theoretical Teaching; TP – Theoretical/ Practical Teaching; TC – Field Work; PL – Theoretical/ Practical Teaching; S – Seminar; OT – Tutor Group; ** – Course Unit available in both semesters; Semestre 2 - 1;Keywords: curriculum, syllabus, program overview, academic plan, course structure, degree requirements, credit distribution, module list, subject breakdown, learning outcomes, ECTS allocation, semester planning, course roadmap, educational objectives, program outline, instructional content, course progression, academic curriculum, study track, course catalog, study plan
-Metadata: {'course_name': 'Data Science', 'degree': 'bachelor', 'doc_type': 'study_plan', 'id': 'c085af09-e2ca-4434-a7a5-65d923355fda', 'source': 'bachelor_data-science_studyplan_text.txt'}</t>
-  </si>
-  <si>
     <t>How does the Master in Information Management, with a specialization in Business Intelligence prepare students for the digital transformation of businesses?</t>
   </si>
   <si>
@@ -1500,12 +1462,60 @@
     <t xml:space="preserve">The Master Degree in Law and Financial Markets is a 4-semester program (120 ECTS) offered by NOVA School of Law, with classes held 2-3 times a week. It is designed for holders of a bachelor's degree (or equivalent) in Law, with a strong emphasis on providing specialized training in areas closely linked to financial markets and investments. The program includes courses on financial markets, risk management, and regulatory frameworks, aiming to equip students with the necessary skills to analyze and evaluate financial instruments, identify strategic interventions in capital markets, and develop a critical approach to solving complex problems. Throughout the program, students can participate in internships, networking events, and international experiences, fostering their professional development and connections within the financial sector. Applications for this program are open until February 28th, 2025.
 </t>
   </si>
+  <si>
+    <t>The course units for the Spring semester of the postgraduate program in Risk Analysis and Management are:
+* Banking and Insurance Regulation and Supervision (Mandatory, 7.5 ECTS)
+* Credit Risk Management (Mandatory, 3.5 ECTS)
+* Financial Derivatives and Risk Management (Mandatory, 7.5 ECTS)
+* Market and Liquidity Risk Management (Mandatory, 4 ECTS)
+* Analysis of Discrete Data (Elective, 4 ECTS)
+* Analysis of Variance (Elective, 4 ECTS)
+* Architectures for Information Systems (Elective, 3.5 ECTS)
+* Big Data Analytics (Elective, 7.5 ECTS)
+* Blockchain (Elective, 4 ECTS)
+* Blockchain &amp; CryptoAssets (Elective, 4 ECTS)
+* Business Impact of Digital Projects (Elective, 3.5 ECTS)
+* Business Intelligence II (Elective, 7.5 ECTS)
+* Computational Statistics II (Elective, 6 ECTS)
+* Customer Relationship Management Systems (Elective, 7.5 ECTS)
+* Cybersecurity (Elective, 7.5 ECTS)
+* Data Mining II (Elective, 7.5 ECTS)
+* Data Visualization (Elective, 7.5 ECTS)
+* Data-driven decision making (Elective, 4 ECTS)
+* E-Business (Elective, 4 ECTS)
+* Econometrics Methods (Elective, 7.5 ECTS)
+* Emerging Technologies for Innovation (Elective, 3.5 ECTS)
+* Enterprise Cloud Mobility (Elective, 7.5 ECTS)
+* Financial Reporting (Elective, 6 ECTS)
+* Gestão do Conhecimento (Elective, 3.5 ECTS)
+* Industry 4.0 (Elective, 4 ECTS)
+* Information Project Management (Elective, 4 ECTS)
+* Innovation Management and Design Thinking (Elective, 7.5 ECTS)
+* Knowledge Management (Elective, 7.5 ECTS)
+* Leadership and People Management (Elective, 7.5 ECTS)
+* Process Mining Powered By Nokia (Elective, 7.5 ECTS)
+* Sampling Theory and Methods (Elective, 7.5 ECTS)
+* Smart and Sustainable Cities (Elective, 7.5 ECTS)
+Please note that this list only includes the course units for the Spring semester and does not include the course units for the other semesters. For a complete overview of the program, I recommend visiting the official course page.</t>
+  </si>
+  <si>
+    <t>GERAR NOVAMENTE</t>
+  </si>
+  <si>
+    <t>TROCAR PARA O MEDIUM</t>
+  </si>
+  <si>
+    <t>Average Faithfulness score</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1518,13 +1528,27 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1554,7 +1578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1566,6 +1590,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,19 +1896,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="113.109375" customWidth="1"/>
-    <col min="2" max="2" width="78.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1893,8 +1925,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1907,22 +1942,28 @@
       <c r="D2">
         <v>234.2156810760498</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3">
         <v>276.47696661949158</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1935,36 +1976,45 @@
       <c r="D4">
         <v>316.33793067932129</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>326.10568165779108</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E5" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>247.00776791572571</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1977,8 +2027,11 @@
       <c r="D7">
         <v>676.13030505180359</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="E7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1991,8 +2044,11 @@
       <c r="D8">
         <v>858.67821168899536</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -2005,621 +2061,739 @@
       <c r="D9">
         <v>430.09221577644348</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
       </c>
       <c r="D10">
         <v>762.26887822151184</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
       </c>
       <c r="D11">
         <v>354.44882678985601</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
       </c>
       <c r="D12">
         <v>219.75348258018491</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
       <c r="D13">
         <v>235.66869592666629</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
       <c r="D14">
         <v>261.47661709785501</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
       </c>
       <c r="D15">
         <v>219.47661709785501</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
       <c r="D16">
         <v>304.52134251594538</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
       <c r="D17">
         <v>181.91693735122681</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
       <c r="D18">
         <v>252.12889766693121</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
       </c>
       <c r="D19">
         <v>176.30128026008609</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
       </c>
       <c r="D20">
         <v>141.36673164367679</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
       </c>
       <c r="D21">
         <v>167.99784851074219</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
       </c>
       <c r="D22">
         <v>220.1376941204071</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
       </c>
       <c r="D23">
         <v>165.95457911491391</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
         <v>69</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>70</v>
-      </c>
-      <c r="C24" t="s">
-        <v>71</v>
       </c>
       <c r="D24">
         <v>175.13230609893799</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>73</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
       </c>
       <c r="D25">
         <v>164.52880072593689</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>76</v>
-      </c>
-      <c r="C26" t="s">
-        <v>77</v>
       </c>
       <c r="D26">
         <v>340.68654370307922</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="6">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
         <v>78</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>79</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
       </c>
       <c r="D27">
         <v>266.64820885658258</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
       </c>
       <c r="D28">
         <v>210.00087261199951</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>85</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
       </c>
       <c r="D29">
         <v>412.91840028762817</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="s">
         <v>87</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>88</v>
-      </c>
-      <c r="C30" t="s">
-        <v>89</v>
       </c>
       <c r="D30">
         <v>1363.628142118454</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="E30" s="6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" s="3">
+        <v>256.21787214279999</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>91</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="D31">
-        <v>185.7060534954071</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32">
+        <v>284.7644829750061</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33">
+        <v>405.5852358341217</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34">
+        <v>474.60538673400902</v>
+      </c>
+      <c r="E34" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35">
+        <v>213.60538673400899</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36">
+        <v>359.02475118637079</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37">
+        <v>220.6621239185333</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38">
+        <v>206.78005528450009</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39">
+        <v>357.05228281021118</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40">
+        <v>242.14848017692569</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41">
+        <v>258.50947427749628</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42">
+        <v>278.30897164344788</v>
+      </c>
+      <c r="E42" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43">
+        <v>263.60844230651861</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44">
+        <v>303.60838317871088</v>
+      </c>
+      <c r="E44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45">
+        <v>294.588801383972</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" s="3">
+        <v>292.80686187743999</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47">
+        <v>234.45348143577581</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="5">
+        <v>186.14145016670199</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="3">
-        <v>256.21787214279999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33">
-        <v>284.7644829750061</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34">
-        <v>405.5852358341217</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35">
-        <v>474.60538673400902</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>103</v>
-      </c>
-      <c r="B36" s="2" t="s">
+    </row>
+    <row r="49" spans="1:5" s="3" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D49" s="3">
+        <v>335.71868515015001</v>
+      </c>
+      <c r="E49" s="6">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50">
+        <v>392.9086811542511</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51">
+        <v>307.90704655647278</v>
+      </c>
+      <c r="E51" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="5">
+        <v>259.27551078796392</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="C36" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36">
-        <v>213.60538673400899</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37">
-        <v>359.02475118637079</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38">
-        <v>220.6621239185333</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39">
-        <v>206.78005528450009</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40">
-        <v>357.05228281021118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41">
-        <v>242.14848017692569</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42">
-        <v>258.50947427749628</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43">
-        <v>278.30897164344788</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" t="s">
-        <v>128</v>
-      </c>
-      <c r="D44">
-        <v>263.60844230651861</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>129</v>
-      </c>
-      <c r="B45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" t="s">
-        <v>131</v>
-      </c>
-      <c r="D45">
-        <v>303.60838317871088</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" t="s">
-        <v>133</v>
-      </c>
-      <c r="C46" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46">
-        <v>294.588801383972</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="3">
-        <v>292.80686187743999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>138</v>
-      </c>
-      <c r="B48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" t="s">
-        <v>140</v>
-      </c>
-      <c r="D48">
-        <v>234.45348143577581</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D49">
-        <v>186.1414501667023</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D50" s="3">
-        <v>335.71868515015001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" t="s">
-        <v>146</v>
-      </c>
-      <c r="C51" t="s">
-        <v>137</v>
-      </c>
-      <c r="D51">
-        <v>392.9086811542511</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>147</v>
-      </c>
-      <c r="B52" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" t="s">
-        <v>149</v>
-      </c>
-      <c r="D52">
-        <v>307.90704655647278</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>150</v>
-      </c>
-      <c r="B53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C53" t="s">
-        <v>152</v>
-      </c>
-      <c r="D53">
-        <v>259.27551078796392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>